<commit_message>
Current progress on Seabloom data
Waiting for response from Eric before finalizing parameters.
</commit_message>
<xml_diff>
--- a/parameternotes/parameters.xlsx
+++ b/parameternotes/parameters.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16280" yWindow="0" windowWidth="34920" windowHeight="19980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
     <sheet name="params" sheetId="1" r:id="rId2"/>
     <sheet name="papers_checked" sheetId="4" r:id="rId3"/>
     <sheet name="HilleRisLambers2010_data" sheetId="6" r:id="rId4"/>
-    <sheet name="HarpoleTilman2006" sheetId="5" r:id="rId5"/>
-    <sheet name="scratch" sheetId="3" r:id="rId6"/>
+    <sheet name="Seabloom2003_data" sheetId="7" r:id="rId5"/>
+    <sheet name="HarpoleTilman2006" sheetId="5" r:id="rId6"/>
+    <sheet name="scratch" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="285">
   <si>
     <t>Parameter</t>
   </si>
@@ -891,6 +892,39 @@
   </si>
   <si>
     <t>from DataScript_CAData_09152016 (Allseed/Allbio)</t>
+  </si>
+  <si>
+    <t>biomass (per individual, estimated across treatment plots)</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>from invade-exp-ann-seed-analysis.R</t>
+  </si>
+  <si>
+    <t>DatafromSeabloom</t>
+  </si>
+  <si>
+    <t>Estimate (mean_across_treatments)</t>
+  </si>
+  <si>
+    <t>Estimate_additional1(min)</t>
+  </si>
+  <si>
+    <t>Estimate_additional_OR_range(max)</t>
+  </si>
+  <si>
+    <t>See R code, this is still in progress!</t>
+  </si>
+  <si>
+    <t>phi (but not including overwintering)</t>
+  </si>
+  <si>
+    <t>seed number per unit total (aboveground) biomass</t>
+  </si>
+  <si>
+    <t>Also, above values of biomass may be wrong too. ..</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1025,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="513">
+  <cellStyleXfs count="547">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1505,8 +1539,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1523,8 +1591,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="513">
+  <cellStyles count="547">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1781,6 +1852,23 @@
     <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2037,6 +2125,23 @@
     <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2492,9 +2597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J131" sqref="J131:J141"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J64" sqref="H64:J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6829,8 +6934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A10" sqref="A2:XFD10"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9899,6 +10004,338 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="16" customFormat="1" ht="68" customHeight="1">
+      <c r="A1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2">
+        <v>1.0803200000000001E-3</v>
+      </c>
+      <c r="E2">
+        <v>7.7499999999999997E-4</v>
+      </c>
+      <c r="F2">
+        <v>1.274E-3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>277</v>
+      </c>
+      <c r="J2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3">
+        <v>1.229873E-3</v>
+      </c>
+      <c r="E3">
+        <v>9.9183330000000001E-4</v>
+      </c>
+      <c r="F3">
+        <v>1.8749999999999999E-3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>275</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>277</v>
+      </c>
+      <c r="J3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4">
+        <v>1.8402830000000001E-3</v>
+      </c>
+      <c r="E4">
+        <v>1.1916379E-3</v>
+      </c>
+      <c r="F4">
+        <v>2.5249999999999999E-3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>275</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>277</v>
+      </c>
+      <c r="J4" t="s">
+        <v>170</v>
+      </c>
+      <c r="K4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6">
+        <v>0.2588047</v>
+      </c>
+      <c r="E6">
+        <v>9.8206000000000002E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.84537499999999999</v>
+      </c>
+      <c r="G6" t="s">
+        <v>275</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>277</v>
+      </c>
+      <c r="J6" t="s">
+        <v>170</v>
+      </c>
+      <c r="K6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D7">
+        <v>0.3110349</v>
+      </c>
+      <c r="E7">
+        <v>8.0433329999999997E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="G7" t="s">
+        <v>275</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>277</v>
+      </c>
+      <c r="J7" t="s">
+        <v>170</v>
+      </c>
+      <c r="K7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D8">
+        <v>0.59340959999999998</v>
+      </c>
+      <c r="E8">
+        <v>0.15483332999999999</v>
+      </c>
+      <c r="F8">
+        <v>1.6617649999999999</v>
+      </c>
+      <c r="G8" t="s">
+        <v>275</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>277</v>
+      </c>
+      <c r="J8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B10" t="s">
+        <v>282</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10">
+        <v>0.3395976</v>
+      </c>
+      <c r="E10">
+        <v>0.1913398</v>
+      </c>
+      <c r="F10">
+        <v>0.4388357</v>
+      </c>
+      <c r="G10" t="s">
+        <v>268</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="C11" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D11">
+        <v>0.4480208</v>
+      </c>
+      <c r="E11">
+        <v>0.34707179999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.54593840000000005</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="C12" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12">
+        <v>0.42446149999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.38145560000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.51464200000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10148,7 +10585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Best calculation of phi that I can muster
</commit_message>
<xml_diff>
--- a/parameternotes/parameters.xlsx
+++ b/parameternotes/parameters.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="10220" yWindow="6420" windowWidth="34140" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,8 @@
     <sheet name="HilleRisLambers2010_data" sheetId="6" r:id="rId4"/>
     <sheet name="Seabloom2003_data" sheetId="7" r:id="rId5"/>
     <sheet name="HarpoleTilman2006" sheetId="5" r:id="rId6"/>
-    <sheet name="scratch" sheetId="3" r:id="rId7"/>
+    <sheet name="quick_phi" sheetId="8" r:id="rId7"/>
+    <sheet name="scratch" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="289">
   <si>
     <t>Parameter</t>
   </si>
@@ -925,6 +926,18 @@
   </si>
   <si>
     <t>Also, above values of biomass may be wrong too. ..</t>
+  </si>
+  <si>
+    <t>est_phi</t>
+  </si>
+  <si>
+    <t>On 29.August.2018:</t>
+  </si>
+  <si>
+    <t>Megan and I created quick_phi to estimate some phi values for our Mayan megadroughts project.</t>
+  </si>
+  <si>
+    <t>We used Janneke's data in gram units (pasted from HilleRisLambers2010_data tab, note that you have to paste the g seed mass, not the mg one).</t>
   </si>
 </sst>
 </file>
@@ -1025,8 +1038,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="547">
+  <cellStyleXfs count="567">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1595,7 +1628,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="547">
+  <cellStyles count="567">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1869,6 +1902,16 @@
     <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2142,6 +2185,16 @@
     <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2473,8 +2526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2577,6 +2630,21 @@
     <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="33" spans="1:1">
@@ -2597,14 +2665,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J64" sqref="H64:J64"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="53.83203125" customWidth="1"/>
+    <col min="1" max="1" width="52.1640625" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="54.6640625" customWidth="1"/>
@@ -6934,8 +7002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8594,7 +8662,7 @@
         <v>250</v>
       </c>
       <c r="D53">
-        <f t="shared" si="1"/>
+        <f>L53*1000</f>
         <v>1.008</v>
       </c>
       <c r="G53" s="8" t="s">
@@ -10006,8 +10074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10339,7 +10407,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10587,6 +10655,495 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>156</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0.10801239999999999</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K2">
+        <v>6.7260000000000002E-3</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O2">
+        <f>D2/K2</f>
+        <v>16.058935474278915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.61728799999999995</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J3" t="s">
+        <v>247</v>
+      </c>
+      <c r="K3">
+        <v>2.0617999999999999E-3</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O11" si="0">D3/K3</f>
+        <v>299.3927636046173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1.8045811</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J4" t="s">
+        <v>236</v>
+      </c>
+      <c r="K4">
+        <v>2.2239999999999998E-3</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>811.41236510791373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.37540839999999998</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J5" t="s">
+        <v>159</v>
+      </c>
+      <c r="K5">
+        <v>2.8350000000000001E-4</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>1324.1918871252203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1.1106361</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J6" t="s">
+        <v>248</v>
+      </c>
+      <c r="K6">
+        <v>3.2939999999999998E-4</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>3371.6942926533093</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.26277660000000003</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J7" t="s">
+        <v>238</v>
+      </c>
+      <c r="K7">
+        <v>4.0733000000000002E-3</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>64.511968183045695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.484655</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J8" t="s">
+        <v>249</v>
+      </c>
+      <c r="K8">
+        <v>4.7839999999999997E-4</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>1013.0748327759198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.41965340000000001</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J9" t="s">
+        <v>250</v>
+      </c>
+      <c r="K9">
+        <v>1.008E-3</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>416.32281746031748</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.3505395</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J10" t="s">
+        <v>251</v>
+      </c>
+      <c r="K10">
+        <v>1.4779999999999999E-3</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>237.17151556156969</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.3505395</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J11" t="s">
+        <v>252</v>
+      </c>
+      <c r="K11">
+        <v>4.28E-4</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>819.01752336448601</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0.55182059999999999</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="J12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K12">
+        <v>3.479E-4</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="O12">
+        <f>D12/K12</f>
+        <v>1586.1471687266455</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
updating analyses from today's work
...hoping for great things tomorrow!
</commit_message>
<xml_diff>
--- a/parameternotes/parameters.xlsx
+++ b/parameternotes/parameters.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2150" uniqueCount="290">
   <si>
     <t>Parameter</t>
   </si>
@@ -938,6 +938,32 @@
   </si>
   <si>
     <t>We used Janneke's data in gram units (pasted from HilleRisLambers2010_data tab, note that you have to paste the g seed mass, not the mg one).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I pulled </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>survivorship</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from GodoyLevine 2014 Appendix B (maybe not included in this Excel file, should check!)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2527,7 +2553,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2645,6 +2671,11 @@
     <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>288</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:1">
@@ -2666,7 +2697,7 @@
   <dimension ref="A1:L141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD75"/>
     </sheetView>
   </sheetViews>

</xml_diff>